<commit_message>
maintain the xls files
</commit_message>
<xml_diff>
--- a/CrowdSourcingStudy/Dialogues_test/Dialogues with exit condition/dialoguesCrows/Dom_D1_Sub_Da.xlsx
+++ b/CrowdSourcingStudy/Dialogues_test/Dialogues with exit condition/dialoguesCrows/Dom_D1_Sub_Da.xlsx
@@ -21,18 +21,13 @@
     <t>content</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "What kind of food do you like?" &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;:"Italian is my favorite food." &lt;br&gt;
-&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Italian is my least preferred food." &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "Let's eat Turkish food tonight." &lt;br&gt;
-&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Sorry, I'd rather choose something else." &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "I prefer Italian food over Japanese." &lt;br&gt;
-&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "I prefer Japanese food over Italian." &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "Let's eat French food tonight." &lt;br&gt;
-&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Okay, let's choose French food." &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "Let's go to the Le Gramophone Restaurant." &lt;br&gt;
-&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Sorry, I'd rather choose something else." &lt;br&gt;
- &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;:"Sorry, but I no longer want to go for dinner!!" &lt;/b&gt;</t>
+    <t>&lt;b&gt;&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Let's eat Chinese food tonight." &lt;br&gt;
+ &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "I like Italian food more than Chinese food. "
+&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Let's go to the Samura restaurant." &lt;br&gt; 
+ &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "I prefer cheap restaurants." &lt;br&gt;
+&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Let's go to the Ying restaurant." &lt;br&gt; 
+ &lt;br&gt;&amp;nbsp&amp;nbsp&amp;nbsp&amp;nbsp&lt;b&gt;B&lt;/b&gt;: "Okay, I'll call to book a table." &lt;br&gt;
+&lt;br&gt;&lt;b&gt;A&lt;/b&gt;: "Ok." &lt;br&gt;&lt;/b&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>